<commit_message>
dp grid problems completed
</commit_message>
<xml_diff>
--- a/Strivers List + other Problems.xlsx
+++ b/Strivers List + other Problems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DSA Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E297641-278A-4E41-8E0C-419D8C02A261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E87E39-E071-4352-8ABE-E017DB003E5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="498">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1059" uniqueCount="500">
   <si>
     <t>Mark as Done</t>
   </si>
@@ -1527,6 +1527,12 @@
   </si>
   <si>
     <t>Minimum path Falling Sum</t>
+  </si>
+  <si>
+    <t>Cherry Pickup 2</t>
+  </si>
+  <si>
+    <t>Devisors of a Number</t>
   </si>
 </sst>
 </file>
@@ -1808,7 +1814,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1977,6 +1983,9 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2214,11 +2223,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Y1070"/>
+  <dimension ref="A1:Y1071"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="102" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A251" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B262" sqref="B262"/>
+      <pane ySplit="4" topLeftCell="A218" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E299" sqref="E299"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -12003,7 +12012,9 @@
       <c r="B260" s="50" t="b">
         <v>1</v>
       </c>
-      <c r="C260" s="2"/>
+      <c r="C260" s="2">
+        <v>9</v>
+      </c>
       <c r="D260" s="1" t="s">
         <v>495</v>
       </c>
@@ -12038,7 +12049,9 @@
       <c r="B261" s="50" t="b">
         <v>1</v>
       </c>
-      <c r="C261" s="2"/>
+      <c r="C261" s="2">
+        <v>10</v>
+      </c>
       <c r="D261" s="1" t="s">
         <v>496</v>
       </c>
@@ -12071,7 +12084,9 @@
       <c r="B262" s="50" t="b">
         <v>1</v>
       </c>
-      <c r="C262" s="2"/>
+      <c r="C262" s="2">
+        <v>11</v>
+      </c>
       <c r="D262" s="1" t="s">
         <v>497</v>
       </c>
@@ -12100,26 +12115,24 @@
       <c r="Y262" s="1"/>
     </row>
     <row r="263" spans="1:25" ht="15" x14ac:dyDescent="0.35">
-      <c r="A263" s="56"/>
+      <c r="A263" s="65"/>
       <c r="B263" s="50" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C263" s="2">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D263" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E263" s="8" t="s">
+        <v>498</v>
+      </c>
+      <c r="E263" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="F263" s="54" t="s">
-        <v>22</v>
+      <c r="F263" s="67" t="s">
+        <v>53</v>
       </c>
       <c r="G263" s="3"/>
-      <c r="H263" s="15" t="s">
-        <v>307</v>
-      </c>
+      <c r="H263" s="15"/>
       <c r="I263" s="3"/>
       <c r="J263" s="1"/>
       <c r="K263" s="1"/>
@@ -12138,26 +12151,26 @@
       <c r="X263" s="1"/>
       <c r="Y263" s="1"/>
     </row>
-    <row r="264" spans="1:25" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:25" ht="15" x14ac:dyDescent="0.35">
       <c r="A264" s="56"/>
       <c r="B264" s="50" t="b">
         <v>0</v>
       </c>
       <c r="C264" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D264" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="E264" s="46" t="s">
+        <v>306</v>
+      </c>
+      <c r="E264" s="8" t="s">
         <v>9</v>
       </c>
       <c r="F264" s="54" t="s">
         <v>22</v>
       </c>
       <c r="G264" s="3"/>
-      <c r="H264" s="16" t="s">
-        <v>309</v>
+      <c r="H264" s="15" t="s">
+        <v>307</v>
       </c>
       <c r="I264" s="3"/>
       <c r="J264" s="1"/>
@@ -12183,12 +12196,12 @@
         <v>0</v>
       </c>
       <c r="C265" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D265" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="E265" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="E265" s="46" t="s">
         <v>9</v>
       </c>
       <c r="F265" s="54" t="s">
@@ -12196,7 +12209,7 @@
       </c>
       <c r="G265" s="3"/>
       <c r="H265" s="16" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="I265" s="3"/>
       <c r="J265" s="1"/>
@@ -12216,16 +12229,16 @@
       <c r="X265" s="1"/>
       <c r="Y265" s="1"/>
     </row>
-    <row r="266" spans="1:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:25" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A266" s="56"/>
       <c r="B266" s="50" t="b">
         <v>0</v>
       </c>
       <c r="C266" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D266" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E266" s="8" t="s">
         <v>9</v>
@@ -12234,8 +12247,8 @@
         <v>22</v>
       </c>
       <c r="G266" s="3"/>
-      <c r="H266" s="15" t="s">
-        <v>313</v>
+      <c r="H266" s="16" t="s">
+        <v>311</v>
       </c>
       <c r="I266" s="3"/>
       <c r="J266" s="1"/>
@@ -12261,10 +12274,10 @@
         <v>0</v>
       </c>
       <c r="C267" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D267" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E267" s="8" t="s">
         <v>9</v>
@@ -12274,7 +12287,7 @@
       </c>
       <c r="G267" s="3"/>
       <c r="H267" s="15" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="I267" s="3"/>
       <c r="J267" s="1"/>
@@ -12300,10 +12313,10 @@
         <v>0</v>
       </c>
       <c r="C268" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D268" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E268" s="8" t="s">
         <v>9</v>
@@ -12313,7 +12326,7 @@
       </c>
       <c r="G268" s="3"/>
       <c r="H268" s="15" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="I268" s="3"/>
       <c r="J268" s="1"/>
@@ -12333,16 +12346,16 @@
       <c r="X268" s="1"/>
       <c r="Y268" s="1"/>
     </row>
-    <row r="269" spans="1:25" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:25" ht="15" x14ac:dyDescent="0.35">
       <c r="A269" s="56"/>
       <c r="B269" s="50" t="b">
         <v>0</v>
       </c>
       <c r="C269" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D269" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E269" s="8" t="s">
         <v>9</v>
@@ -12351,8 +12364,8 @@
         <v>22</v>
       </c>
       <c r="G269" s="3"/>
-      <c r="H269" s="16" t="s">
-        <v>319</v>
+      <c r="H269" s="15" t="s">
+        <v>317</v>
       </c>
       <c r="I269" s="3"/>
       <c r="J269" s="1"/>
@@ -12372,16 +12385,16 @@
       <c r="X269" s="1"/>
       <c r="Y269" s="1"/>
     </row>
-    <row r="270" spans="1:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:25" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A270" s="56"/>
       <c r="B270" s="50" t="b">
         <v>0</v>
       </c>
       <c r="C270" s="2">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D270" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E270" s="8" t="s">
         <v>9</v>
@@ -12390,8 +12403,8 @@
         <v>22</v>
       </c>
       <c r="G270" s="3"/>
-      <c r="H270" s="15" t="s">
-        <v>321</v>
+      <c r="H270" s="16" t="s">
+        <v>319</v>
       </c>
       <c r="I270" s="3"/>
       <c r="J270" s="1"/>
@@ -12417,10 +12430,10 @@
         <v>0</v>
       </c>
       <c r="C271" s="2">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D271" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E271" s="8" t="s">
         <v>9</v>
@@ -12430,7 +12443,7 @@
       </c>
       <c r="G271" s="3"/>
       <c r="H271" s="15" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="I271" s="3"/>
       <c r="J271" s="1"/>
@@ -12450,16 +12463,16 @@
       <c r="X271" s="1"/>
       <c r="Y271" s="1"/>
     </row>
-    <row r="272" spans="1:25" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:25" ht="15" x14ac:dyDescent="0.35">
       <c r="A272" s="56"/>
       <c r="B272" s="50" t="b">
         <v>0</v>
       </c>
       <c r="C272" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D272" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="E272" s="8" t="s">
         <v>9</v>
@@ -12468,8 +12481,8 @@
         <v>22</v>
       </c>
       <c r="G272" s="3"/>
-      <c r="H272" s="16" t="s">
-        <v>325</v>
+      <c r="H272" s="15" t="s">
+        <v>323</v>
       </c>
       <c r="I272" s="3"/>
       <c r="J272" s="1"/>
@@ -12489,16 +12502,16 @@
       <c r="X272" s="1"/>
       <c r="Y272" s="1"/>
     </row>
-    <row r="273" spans="1:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:25" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A273" s="56"/>
       <c r="B273" s="50" t="b">
         <v>0</v>
       </c>
       <c r="C273" s="2">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D273" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="E273" s="8" t="s">
         <v>9</v>
@@ -12507,8 +12520,8 @@
         <v>22</v>
       </c>
       <c r="G273" s="3"/>
-      <c r="H273" s="15" t="s">
-        <v>327</v>
+      <c r="H273" s="16" t="s">
+        <v>325</v>
       </c>
       <c r="I273" s="3"/>
       <c r="J273" s="1"/>
@@ -12534,10 +12547,10 @@
         <v>0</v>
       </c>
       <c r="C274" s="2">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D274" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E274" s="8" t="s">
         <v>9</v>
@@ -12547,7 +12560,7 @@
       </c>
       <c r="G274" s="3"/>
       <c r="H274" s="15" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="I274" s="3"/>
       <c r="J274" s="1"/>
@@ -12573,10 +12586,10 @@
         <v>0</v>
       </c>
       <c r="C275" s="2">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D275" s="1" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="E275" s="8" t="s">
         <v>9</v>
@@ -12586,7 +12599,7 @@
       </c>
       <c r="G275" s="3"/>
       <c r="H275" s="15" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="I275" s="3"/>
       <c r="J275" s="1"/>
@@ -12606,16 +12619,16 @@
       <c r="X275" s="1"/>
       <c r="Y275" s="1"/>
     </row>
-    <row r="276" spans="1:25" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:25" ht="15" x14ac:dyDescent="0.35">
       <c r="A276" s="56"/>
       <c r="B276" s="50" t="b">
         <v>0</v>
       </c>
       <c r="C276" s="2">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D276" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="E276" s="8" t="s">
         <v>9</v>
@@ -12624,8 +12637,8 @@
         <v>22</v>
       </c>
       <c r="G276" s="3"/>
-      <c r="H276" s="16" t="s">
-        <v>333</v>
+      <c r="H276" s="15" t="s">
+        <v>331</v>
       </c>
       <c r="I276" s="3"/>
       <c r="J276" s="1"/>
@@ -12651,20 +12664,20 @@
         <v>0</v>
       </c>
       <c r="C277" s="2">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D277" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="E277" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F277" s="28" t="s">
-        <v>53</v>
+      <c r="F277" s="54" t="s">
+        <v>22</v>
       </c>
       <c r="G277" s="3"/>
       <c r="H277" s="16" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I277" s="3"/>
       <c r="J277" s="1"/>
@@ -12690,10 +12703,10 @@
         <v>0</v>
       </c>
       <c r="C278" s="2">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D278" s="1" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="E278" s="8" t="s">
         <v>9</v>
@@ -12703,7 +12716,7 @@
       </c>
       <c r="G278" s="3"/>
       <c r="H278" s="16" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="I278" s="3"/>
       <c r="J278" s="1"/>
@@ -12729,10 +12742,10 @@
         <v>0</v>
       </c>
       <c r="C279" s="2">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D279" s="1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E279" s="8" t="s">
         <v>9</v>
@@ -12742,7 +12755,7 @@
       </c>
       <c r="G279" s="3"/>
       <c r="H279" s="16" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="I279" s="3"/>
       <c r="J279" s="1"/>
@@ -12762,16 +12775,16 @@
       <c r="X279" s="1"/>
       <c r="Y279" s="1"/>
     </row>
-    <row r="280" spans="1:25" ht="15" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:25" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A280" s="56"/>
       <c r="B280" s="50" t="b">
         <v>0</v>
       </c>
       <c r="C280" s="2">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D280" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E280" s="8" t="s">
         <v>9</v>
@@ -12780,8 +12793,8 @@
         <v>53</v>
       </c>
       <c r="G280" s="3"/>
-      <c r="H280" s="15" t="s">
-        <v>341</v>
+      <c r="H280" s="16" t="s">
+        <v>339</v>
       </c>
       <c r="I280" s="3"/>
       <c r="J280" s="1"/>
@@ -12807,10 +12820,10 @@
         <v>0</v>
       </c>
       <c r="C281" s="2">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D281" s="1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E281" s="8" t="s">
         <v>9</v>
@@ -12820,7 +12833,7 @@
       </c>
       <c r="G281" s="3"/>
       <c r="H281" s="15" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="I281" s="3"/>
       <c r="J281" s="1"/>
@@ -12840,16 +12853,16 @@
       <c r="X281" s="1"/>
       <c r="Y281" s="1"/>
     </row>
-    <row r="282" spans="1:25" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:25" ht="15" x14ac:dyDescent="0.35">
       <c r="A282" s="56"/>
       <c r="B282" s="50" t="b">
         <v>0</v>
       </c>
       <c r="C282" s="2">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D282" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E282" s="8" t="s">
         <v>9</v>
@@ -12858,8 +12871,8 @@
         <v>53</v>
       </c>
       <c r="G282" s="3"/>
-      <c r="H282" s="16" t="s">
-        <v>345</v>
+      <c r="H282" s="15" t="s">
+        <v>343</v>
       </c>
       <c r="I282" s="3"/>
       <c r="J282" s="1"/>
@@ -12879,15 +12892,27 @@
       <c r="X282" s="1"/>
       <c r="Y282" s="1"/>
     </row>
-    <row r="283" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A283" s="1"/>
-      <c r="B283" s="1"/>
-      <c r="C283" s="2"/>
-      <c r="D283" s="1"/>
-      <c r="E283" s="3"/>
-      <c r="F283" s="1"/>
+    <row r="283" spans="1:25" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A283" s="56"/>
+      <c r="B283" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="C283" s="2">
+        <v>23</v>
+      </c>
+      <c r="D283" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="E283" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F283" s="28" t="s">
+        <v>53</v>
+      </c>
       <c r="G283" s="3"/>
-      <c r="H283" s="4"/>
+      <c r="H283" s="16" t="s">
+        <v>345</v>
+      </c>
       <c r="I283" s="3"/>
       <c r="J283" s="1"/>
       <c r="K283" s="1"/>
@@ -12933,29 +12958,15 @@
       <c r="X284" s="1"/>
       <c r="Y284" s="1"/>
     </row>
-    <row r="285" spans="1:25" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A285" s="65" t="s">
-        <v>346</v>
-      </c>
-      <c r="B285" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="C285" s="2">
-        <v>1</v>
-      </c>
-      <c r="D285" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="E285" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="F285" s="27" t="s">
-        <v>10</v>
-      </c>
+    <row r="285" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A285" s="1"/>
+      <c r="B285" s="1"/>
+      <c r="C285" s="2"/>
+      <c r="D285" s="1"/>
+      <c r="E285" s="3"/>
+      <c r="F285" s="1"/>
       <c r="G285" s="3"/>
-      <c r="H285" s="16" t="s">
-        <v>348</v>
-      </c>
+      <c r="H285" s="4"/>
       <c r="I285" s="3"/>
       <c r="J285" s="1"/>
       <c r="K285" s="1"/>
@@ -12974,26 +12985,28 @@
       <c r="X285" s="1"/>
       <c r="Y285" s="1"/>
     </row>
-    <row r="286" spans="1:25" ht="15" x14ac:dyDescent="0.35">
-      <c r="A286" s="56"/>
+    <row r="286" spans="1:25" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A286" s="65" t="s">
+        <v>346</v>
+      </c>
       <c r="B286" s="50" t="b">
         <v>0</v>
       </c>
       <c r="C286" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D286" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="E286" s="8" t="s">
+        <v>347</v>
+      </c>
+      <c r="E286" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="F286" s="26" t="s">
-        <v>22</v>
+      <c r="F286" s="27" t="s">
+        <v>10</v>
       </c>
       <c r="G286" s="3"/>
-      <c r="H286" s="15" t="s">
-        <v>350</v>
+      <c r="H286" s="16" t="s">
+        <v>348</v>
       </c>
       <c r="I286" s="3"/>
       <c r="J286" s="1"/>
@@ -13019,10 +13032,10 @@
         <v>0</v>
       </c>
       <c r="C287" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D287" s="1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="E287" s="8" t="s">
         <v>9</v>
@@ -13032,7 +13045,7 @@
       </c>
       <c r="G287" s="3"/>
       <c r="H287" s="15" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="I287" s="3"/>
       <c r="J287" s="1"/>
@@ -13058,10 +13071,10 @@
         <v>0</v>
       </c>
       <c r="C288" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D288" s="1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E288" s="8" t="s">
         <v>9</v>
@@ -13071,7 +13084,7 @@
       </c>
       <c r="G288" s="3"/>
       <c r="H288" s="15" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="I288" s="3"/>
       <c r="J288" s="1"/>
@@ -13097,10 +13110,10 @@
         <v>0</v>
       </c>
       <c r="C289" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D289" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E289" s="8" t="s">
         <v>9</v>
@@ -13109,8 +13122,8 @@
         <v>22</v>
       </c>
       <c r="G289" s="3"/>
-      <c r="H289" s="20" t="s">
-        <v>356</v>
+      <c r="H289" s="15" t="s">
+        <v>354</v>
       </c>
       <c r="I289" s="3"/>
       <c r="J289" s="1"/>
@@ -13136,20 +13149,20 @@
         <v>0</v>
       </c>
       <c r="C290" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D290" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E290" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F290" s="28" t="s">
-        <v>53</v>
+      <c r="F290" s="26" t="s">
+        <v>22</v>
       </c>
       <c r="G290" s="3"/>
-      <c r="H290" s="15" t="s">
-        <v>358</v>
+      <c r="H290" s="20" t="s">
+        <v>356</v>
       </c>
       <c r="I290" s="3"/>
       <c r="J290" s="1"/>
@@ -13169,17 +13182,27 @@
       <c r="X290" s="1"/>
       <c r="Y290" s="1"/>
     </row>
-    <row r="291" spans="1:25" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A291" s="1"/>
+    <row r="291" spans="1:25" ht="15" x14ac:dyDescent="0.35">
+      <c r="A291" s="56"/>
       <c r="B291" s="50" t="b">
         <v>0</v>
       </c>
-      <c r="C291" s="2"/>
-      <c r="D291" s="1"/>
-      <c r="E291" s="3"/>
-      <c r="F291" s="1"/>
+      <c r="C291" s="2">
+        <v>6</v>
+      </c>
+      <c r="D291" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="E291" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F291" s="28" t="s">
+        <v>53</v>
+      </c>
       <c r="G291" s="3"/>
-      <c r="H291" s="4"/>
+      <c r="H291" s="15" t="s">
+        <v>358</v>
+      </c>
       <c r="I291" s="3"/>
       <c r="J291" s="1"/>
       <c r="K291" s="1"/>
@@ -13228,24 +13251,14 @@
       <c r="Y292" s="1"/>
     </row>
     <row r="293" spans="1:25" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A293" s="62" t="s">
-        <v>392</v>
-      </c>
+      <c r="A293" s="1"/>
       <c r="B293" s="50" t="b">
         <v>0</v>
       </c>
-      <c r="C293" s="2">
-        <v>1</v>
-      </c>
-      <c r="D293" s="1" t="s">
-        <v>400</v>
-      </c>
-      <c r="E293" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F293" s="40" t="s">
-        <v>401</v>
-      </c>
+      <c r="C293" s="2"/>
+      <c r="D293" s="1"/>
+      <c r="E293" s="3"/>
+      <c r="F293" s="1"/>
       <c r="G293" s="3"/>
       <c r="H293" s="4"/>
       <c r="I293" s="3"/>
@@ -13267,15 +13280,17 @@
       <c r="Y293" s="1"/>
     </row>
     <row r="294" spans="1:25" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A294" s="56"/>
+      <c r="A294" s="62" t="s">
+        <v>392</v>
+      </c>
       <c r="B294" s="50" t="b">
         <v>0</v>
       </c>
       <c r="C294" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D294" s="1" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="E294" s="21" t="s">
         <v>9</v>
@@ -13309,10 +13324,10 @@
         <v>0</v>
       </c>
       <c r="C295" s="2">
-        <v>3</v>
-      </c>
-      <c r="D295" s="24" t="s">
-        <v>405</v>
+        <v>2</v>
+      </c>
+      <c r="D295" s="1" t="s">
+        <v>403</v>
       </c>
       <c r="E295" s="21" t="s">
         <v>9</v>
@@ -13346,10 +13361,10 @@
         <v>0</v>
       </c>
       <c r="C296" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D296" s="24" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E296" s="21" t="s">
         <v>9</v>
@@ -13380,13 +13395,13 @@
     <row r="297" spans="1:25" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A297" s="56"/>
       <c r="B297" s="50" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C297" s="2">
-        <v>5</v>
-      </c>
-      <c r="D297" s="1" t="s">
-        <v>481</v>
+        <v>4</v>
+      </c>
+      <c r="D297" s="24" t="s">
+        <v>406</v>
       </c>
       <c r="E297" s="21" t="s">
         <v>9</v>
@@ -13417,14 +13432,20 @@
     <row r="298" spans="1:25" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A298" s="56"/>
       <c r="B298" s="50" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C298" s="2">
-        <v>6</v>
-      </c>
-      <c r="D298" s="1"/>
-      <c r="E298" s="3"/>
-      <c r="F298" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="D298" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="E298" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F298" s="40" t="s">
+        <v>401</v>
+      </c>
       <c r="G298" s="3"/>
       <c r="H298" s="4"/>
       <c r="I298" s="3"/>
@@ -13451,10 +13472,14 @@
         <v>0</v>
       </c>
       <c r="C299" s="2">
-        <v>7</v>
-      </c>
-      <c r="D299" s="1"/>
-      <c r="E299" s="3"/>
+        <v>6</v>
+      </c>
+      <c r="D299" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="E299" s="21" t="s">
+        <v>9</v>
+      </c>
       <c r="F299" s="1"/>
       <c r="G299" s="3"/>
       <c r="H299" s="4"/>
@@ -13482,7 +13507,7 @@
         <v>0</v>
       </c>
       <c r="C300" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D300" s="1"/>
       <c r="E300" s="3"/>
@@ -13513,7 +13538,7 @@
         <v>0</v>
       </c>
       <c r="C301" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D301" s="1"/>
       <c r="E301" s="3"/>
@@ -13544,7 +13569,7 @@
         <v>0</v>
       </c>
       <c r="C302" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D302" s="1"/>
       <c r="E302" s="3"/>
@@ -13575,7 +13600,7 @@
         <v>0</v>
       </c>
       <c r="C303" s="2">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D303" s="1"/>
       <c r="E303" s="3"/>
@@ -13606,7 +13631,7 @@
         <v>0</v>
       </c>
       <c r="C304" s="2">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D304" s="1"/>
       <c r="E304" s="3"/>
@@ -13637,7 +13662,7 @@
         <v>0</v>
       </c>
       <c r="C305" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D305" s="1"/>
       <c r="E305" s="3"/>
@@ -13668,7 +13693,7 @@
         <v>0</v>
       </c>
       <c r="C306" s="2">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D306" s="1"/>
       <c r="E306" s="3"/>
@@ -13699,7 +13724,7 @@
         <v>0</v>
       </c>
       <c r="C307" s="2">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D307" s="1"/>
       <c r="E307" s="3"/>
@@ -13724,10 +13749,14 @@
       <c r="X307" s="1"/>
       <c r="Y307" s="1"/>
     </row>
-    <row r="308" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:25" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A308" s="56"/>
-      <c r="B308" s="1"/>
-      <c r="C308" s="2"/>
+      <c r="B308" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="C308" s="2">
+        <v>15</v>
+      </c>
       <c r="D308" s="1"/>
       <c r="E308" s="3"/>
       <c r="F308" s="1"/>
@@ -13860,7 +13889,7 @@
       <c r="Y312" s="1"/>
     </row>
     <row r="313" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A313" s="1"/>
+      <c r="A313" s="56"/>
       <c r="B313" s="1"/>
       <c r="C313" s="2"/>
       <c r="D313" s="1"/>
@@ -34325,16 +34354,43 @@
       <c r="X1070" s="1"/>
       <c r="Y1070" s="1"/>
     </row>
+    <row r="1071" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A1071" s="1"/>
+      <c r="B1071" s="1"/>
+      <c r="C1071" s="2"/>
+      <c r="D1071" s="1"/>
+      <c r="E1071" s="3"/>
+      <c r="F1071" s="1"/>
+      <c r="G1071" s="3"/>
+      <c r="H1071" s="4"/>
+      <c r="I1071" s="3"/>
+      <c r="J1071" s="1"/>
+      <c r="K1071" s="1"/>
+      <c r="L1071" s="1"/>
+      <c r="M1071" s="1"/>
+      <c r="N1071" s="1"/>
+      <c r="O1071" s="1"/>
+      <c r="P1071" s="1"/>
+      <c r="Q1071" s="1"/>
+      <c r="R1071" s="1"/>
+      <c r="S1071" s="1"/>
+      <c r="T1071" s="1"/>
+      <c r="U1071" s="1"/>
+      <c r="V1071" s="1"/>
+      <c r="W1071" s="1"/>
+      <c r="X1071" s="1"/>
+      <c r="Y1071" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="15">
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="A6:A48"/>
     <mergeCell ref="A53:A69"/>
-    <mergeCell ref="A293:A312"/>
+    <mergeCell ref="A294:A313"/>
     <mergeCell ref="A74:A91"/>
     <mergeCell ref="A96:A109"/>
-    <mergeCell ref="A252:A282"/>
-    <mergeCell ref="A285:A290"/>
+    <mergeCell ref="A252:A283"/>
+    <mergeCell ref="A286:A291"/>
     <mergeCell ref="A112:A129"/>
     <mergeCell ref="A132:A148"/>
     <mergeCell ref="A151:A178"/>
@@ -34520,31 +34576,31 @@
     <hyperlink ref="E245" r:id="rId174" xr:uid="{00000000-0004-0000-0000-0000EE000000}"/>
     <hyperlink ref="E247" r:id="rId175" xr:uid="{00000000-0004-0000-0000-0000EF000000}"/>
     <hyperlink ref="E248" r:id="rId176" xr:uid="{00000000-0004-0000-0000-0000F0000000}"/>
-    <hyperlink ref="E264" r:id="rId177" xr:uid="{00000000-0004-0000-0000-0000F3000000}"/>
-    <hyperlink ref="E265" r:id="rId178" xr:uid="{00000000-0004-0000-0000-0000F4000000}"/>
-    <hyperlink ref="E266" r:id="rId179" xr:uid="{00000000-0004-0000-0000-0000F5000000}"/>
-    <hyperlink ref="E267" r:id="rId180" xr:uid="{00000000-0004-0000-0000-0000F6000000}"/>
-    <hyperlink ref="E268" r:id="rId181" xr:uid="{00000000-0004-0000-0000-0000F7000000}"/>
-    <hyperlink ref="E269" r:id="rId182" xr:uid="{00000000-0004-0000-0000-0000F8000000}"/>
-    <hyperlink ref="E270" r:id="rId183" xr:uid="{00000000-0004-0000-0000-0000F9000000}"/>
-    <hyperlink ref="E271" r:id="rId184" xr:uid="{00000000-0004-0000-0000-0000FA000000}"/>
-    <hyperlink ref="E272" r:id="rId185" xr:uid="{00000000-0004-0000-0000-0000FB000000}"/>
-    <hyperlink ref="E273" r:id="rId186" xr:uid="{00000000-0004-0000-0000-0000FC000000}"/>
-    <hyperlink ref="E274" r:id="rId187" xr:uid="{00000000-0004-0000-0000-0000FD000000}"/>
-    <hyperlink ref="E275" r:id="rId188" xr:uid="{00000000-0004-0000-0000-0000FE000000}"/>
-    <hyperlink ref="E276" r:id="rId189" xr:uid="{00000000-0004-0000-0000-0000FF000000}"/>
-    <hyperlink ref="E277" r:id="rId190" xr:uid="{00000000-0004-0000-0000-000000010000}"/>
-    <hyperlink ref="E278" r:id="rId191" xr:uid="{00000000-0004-0000-0000-000001010000}"/>
-    <hyperlink ref="E279" r:id="rId192" xr:uid="{00000000-0004-0000-0000-000002010000}"/>
-    <hyperlink ref="E280" r:id="rId193" xr:uid="{00000000-0004-0000-0000-000003010000}"/>
-    <hyperlink ref="E281" r:id="rId194" xr:uid="{00000000-0004-0000-0000-000004010000}"/>
-    <hyperlink ref="E282" r:id="rId195" xr:uid="{00000000-0004-0000-0000-000005010000}"/>
-    <hyperlink ref="E285" r:id="rId196" xr:uid="{00000000-0004-0000-0000-000006010000}"/>
-    <hyperlink ref="E286" r:id="rId197" xr:uid="{00000000-0004-0000-0000-000007010000}"/>
-    <hyperlink ref="E287" r:id="rId198" xr:uid="{00000000-0004-0000-0000-000008010000}"/>
-    <hyperlink ref="E288" r:id="rId199" xr:uid="{00000000-0004-0000-0000-000009010000}"/>
-    <hyperlink ref="E289" r:id="rId200" xr:uid="{00000000-0004-0000-0000-00000A010000}"/>
-    <hyperlink ref="E290" r:id="rId201" xr:uid="{00000000-0004-0000-0000-00000B010000}"/>
+    <hyperlink ref="E265" r:id="rId177" xr:uid="{00000000-0004-0000-0000-0000F3000000}"/>
+    <hyperlink ref="E266" r:id="rId178" xr:uid="{00000000-0004-0000-0000-0000F4000000}"/>
+    <hyperlink ref="E267" r:id="rId179" xr:uid="{00000000-0004-0000-0000-0000F5000000}"/>
+    <hyperlink ref="E268" r:id="rId180" xr:uid="{00000000-0004-0000-0000-0000F6000000}"/>
+    <hyperlink ref="E269" r:id="rId181" xr:uid="{00000000-0004-0000-0000-0000F7000000}"/>
+    <hyperlink ref="E270" r:id="rId182" xr:uid="{00000000-0004-0000-0000-0000F8000000}"/>
+    <hyperlink ref="E271" r:id="rId183" xr:uid="{00000000-0004-0000-0000-0000F9000000}"/>
+    <hyperlink ref="E272" r:id="rId184" xr:uid="{00000000-0004-0000-0000-0000FA000000}"/>
+    <hyperlink ref="E273" r:id="rId185" xr:uid="{00000000-0004-0000-0000-0000FB000000}"/>
+    <hyperlink ref="E274" r:id="rId186" xr:uid="{00000000-0004-0000-0000-0000FC000000}"/>
+    <hyperlink ref="E275" r:id="rId187" xr:uid="{00000000-0004-0000-0000-0000FD000000}"/>
+    <hyperlink ref="E276" r:id="rId188" xr:uid="{00000000-0004-0000-0000-0000FE000000}"/>
+    <hyperlink ref="E277" r:id="rId189" xr:uid="{00000000-0004-0000-0000-0000FF000000}"/>
+    <hyperlink ref="E278" r:id="rId190" xr:uid="{00000000-0004-0000-0000-000000010000}"/>
+    <hyperlink ref="E279" r:id="rId191" xr:uid="{00000000-0004-0000-0000-000001010000}"/>
+    <hyperlink ref="E280" r:id="rId192" xr:uid="{00000000-0004-0000-0000-000002010000}"/>
+    <hyperlink ref="E281" r:id="rId193" xr:uid="{00000000-0004-0000-0000-000003010000}"/>
+    <hyperlink ref="E282" r:id="rId194" xr:uid="{00000000-0004-0000-0000-000004010000}"/>
+    <hyperlink ref="E283" r:id="rId195" xr:uid="{00000000-0004-0000-0000-000005010000}"/>
+    <hyperlink ref="E286" r:id="rId196" xr:uid="{00000000-0004-0000-0000-000006010000}"/>
+    <hyperlink ref="E287" r:id="rId197" xr:uid="{00000000-0004-0000-0000-000007010000}"/>
+    <hyperlink ref="E288" r:id="rId198" xr:uid="{00000000-0004-0000-0000-000008010000}"/>
+    <hyperlink ref="E289" r:id="rId199" xr:uid="{00000000-0004-0000-0000-000009010000}"/>
+    <hyperlink ref="E290" r:id="rId200" xr:uid="{00000000-0004-0000-0000-00000A010000}"/>
+    <hyperlink ref="E291" r:id="rId201" xr:uid="{00000000-0004-0000-0000-00000B010000}"/>
     <hyperlink ref="E249" r:id="rId202" xr:uid="{38535620-DA2F-45B6-BE53-7BE35BAD917E}"/>
     <hyperlink ref="E180" r:id="rId203" xr:uid="{52A62708-7A1B-4947-8125-51CD78E69CDC}"/>
     <hyperlink ref="E179" r:id="rId204" xr:uid="{90A2CCC4-C963-4688-BF93-898F1AB744EB}"/>
@@ -34599,13 +34655,13 @@
     <hyperlink ref="E10" r:id="rId253" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
     <hyperlink ref="G7" r:id="rId254" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
     <hyperlink ref="E7" r:id="rId255" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="E293" r:id="rId256" xr:uid="{49C446A4-86D9-438E-8C85-C2CBF2D0C601}"/>
+    <hyperlink ref="E294" r:id="rId256" xr:uid="{49C446A4-86D9-438E-8C85-C2CBF2D0C601}"/>
     <hyperlink ref="E29" r:id="rId257" xr:uid="{15B4076B-7C29-451C-A0E0-E0CDB84955C7}"/>
-    <hyperlink ref="E294" r:id="rId258" xr:uid="{5897208F-5F6C-4E1B-8B0F-03D62428448A}"/>
+    <hyperlink ref="E295" r:id="rId258" xr:uid="{5897208F-5F6C-4E1B-8B0F-03D62428448A}"/>
     <hyperlink ref="E41" r:id="rId259" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
     <hyperlink ref="E15" r:id="rId260" xr:uid="{36657CEA-F972-477D-AC24-77B031A0C947}"/>
-    <hyperlink ref="E295" r:id="rId261" xr:uid="{0B318E6F-5375-45A5-A623-A5D070F4F786}"/>
-    <hyperlink ref="E296" r:id="rId262" xr:uid="{28A35100-95C6-4598-8EAE-4903F97A507B}"/>
+    <hyperlink ref="E296" r:id="rId261" xr:uid="{0B318E6F-5375-45A5-A623-A5D070F4F786}"/>
+    <hyperlink ref="E297" r:id="rId262" xr:uid="{28A35100-95C6-4598-8EAE-4903F97A507B}"/>
     <hyperlink ref="E32" r:id="rId263" xr:uid="{A642EB9F-9B4D-467C-AA82-CE1A728B251C}"/>
     <hyperlink ref="E27" r:id="rId264" xr:uid="{A1884A7B-6025-4BC0-B0A7-10DF9BA889E7}"/>
     <hyperlink ref="E241" r:id="rId265" xr:uid="{DD148482-9331-495D-A315-B2667528DE27}"/>
@@ -34664,7 +34720,7 @@
     <hyperlink ref="E154" r:id="rId318" xr:uid="{3F9A6173-1CC2-4924-8DCB-DA0907EBC497}"/>
     <hyperlink ref="E23" r:id="rId319" xr:uid="{CFCB346F-57BF-4E1F-A83E-1ECF2056F264}"/>
     <hyperlink ref="E102" r:id="rId320" xr:uid="{2356458E-6B22-49DA-9E6A-10397CF5FFCB}"/>
-    <hyperlink ref="E297" r:id="rId321" xr:uid="{4E26D969-664E-4EA5-BCDD-C0244659BD80}"/>
+    <hyperlink ref="E298" r:id="rId321" xr:uid="{4E26D969-664E-4EA5-BCDD-C0244659BD80}"/>
     <hyperlink ref="E11" r:id="rId322" xr:uid="{79FBDA3E-6FA8-4642-9106-ECA30BC0F184}"/>
     <hyperlink ref="E16" r:id="rId323" xr:uid="{76475329-A2A3-4832-B080-9DF1FCF7B69C}"/>
     <hyperlink ref="E34" r:id="rId324" xr:uid="{712331F6-B9ED-461A-B3A4-361688CBC32C}"/>
@@ -34673,7 +34729,7 @@
     <hyperlink ref="E19" r:id="rId327" xr:uid="{CD31F41D-EA1B-403F-8D0D-B77515C1536B}"/>
     <hyperlink ref="E113" r:id="rId328" xr:uid="{127B98B1-79F3-43C9-B7FF-4FBC27351376}"/>
     <hyperlink ref="E255" r:id="rId329" xr:uid="{2D7D988B-76D9-4BEC-8F29-806C1E841434}"/>
-    <hyperlink ref="E263" r:id="rId330" xr:uid="{00000000-0004-0000-0000-0000F2000000}"/>
+    <hyperlink ref="E264" r:id="rId330" xr:uid="{00000000-0004-0000-0000-0000F2000000}"/>
     <hyperlink ref="E256" r:id="rId331" xr:uid="{243B74CF-B5C2-468E-9F2F-0DA78790403B}"/>
     <hyperlink ref="E257" r:id="rId332" xr:uid="{9E359A2D-80A4-4440-B6F6-E0BD637BE478}"/>
     <hyperlink ref="E259" r:id="rId333" xr:uid="{92D99966-CAE9-4A3E-8110-212EFFA305D9}"/>
@@ -34682,8 +34738,10 @@
     <hyperlink ref="E260" r:id="rId336" xr:uid="{9E27F39A-FC85-46E5-98FF-497FB0860FA7}"/>
     <hyperlink ref="E261" r:id="rId337" xr:uid="{3BF3C81C-57C8-46D6-BC82-B24998AE425F}"/>
     <hyperlink ref="E262" r:id="rId338" xr:uid="{D60890AA-5FFE-44F0-AA27-28E4BFB644F6}"/>
+    <hyperlink ref="E263" r:id="rId339" xr:uid="{BEBCCD33-BF2B-422C-8302-61C8E85BEDED}"/>
+    <hyperlink ref="E299" r:id="rId340" xr:uid="{FC2672B5-6248-497C-B62C-4B7547222ED5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId339"/>
+  <pageSetup orientation="portrait" r:id="rId341"/>
 </worksheet>
 </file>
</xml_diff>